<commit_message>
exam report and full screen scrolling fix
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skuma561\Desktop\ADDA\Code\React\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skuma561\Desktop\ADDA\Code\React\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>QuestionDesc</t>
   </si>
@@ -44,37 +44,133 @@
     <t>answer</t>
   </si>
   <si>
-    <t>Capital City of Manipur</t>
-  </si>
-  <si>
-    <t>Capital City of Meghalaya</t>
-  </si>
-  <si>
-    <t>Itanagar</t>
-  </si>
-  <si>
-    <t>Imphal</t>
-  </si>
-  <si>
-    <t>Shillong</t>
-  </si>
-  <si>
-    <t>Capital City of Bihar</t>
-  </si>
-  <si>
-    <t>Patna</t>
-  </si>
-  <si>
-    <t>Capital City of Rajashtan</t>
-  </si>
-  <si>
-    <t>Jaipur</t>
-  </si>
-  <si>
-    <t>Aizawl</t>
-  </si>
-  <si>
     <t>Sr</t>
+  </si>
+  <si>
+    <t>The 1st person to set foot on Moon was?</t>
+  </si>
+  <si>
+    <t>Nil Armstrong</t>
+  </si>
+  <si>
+    <t>Rakesh Sharma</t>
+  </si>
+  <si>
+    <t>Rayan Prince</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>What Mogul emporer of India from 1556-1605, took the throne at age 13 and was the grandson of Babar?</t>
+  </si>
+  <si>
+    <t> Delhi Sultanate</t>
+  </si>
+  <si>
+    <t>Humayun</t>
+  </si>
+  <si>
+    <t>Abbas the Great</t>
+  </si>
+  <si>
+    <t>Akbar the Great</t>
+  </si>
+  <si>
+    <t>The well-known theorist of New Social Movement is</t>
+  </si>
+  <si>
+    <t>Habermas</t>
+  </si>
+  <si>
+    <t>Karl Marx</t>
+  </si>
+  <si>
+    <t> Foucault</t>
+  </si>
+  <si>
+    <t>Althusser</t>
+  </si>
+  <si>
+    <t>Which was the Napoleon last battle in which he was captured and exiled to St Helena?</t>
+  </si>
+  <si>
+    <t>Battle of Waterloo</t>
+  </si>
+  <si>
+    <t>Battle of France</t>
+  </si>
+  <si>
+    <t>Battle of Paris</t>
+  </si>
+  <si>
+    <t>Battle of London</t>
+  </si>
+  <si>
+    <t>In which year Bangladesh was formed as Separate Country?</t>
+  </si>
+  <si>
+    <t>The longest river in the world is the.</t>
+  </si>
+  <si>
+    <t>Nile</t>
+  </si>
+  <si>
+    <t>Ganga</t>
+  </si>
+  <si>
+    <t>Brhamputra</t>
+  </si>
+  <si>
+    <t> Yamuna</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t> India</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>When was the 1st person to set foot on Moon?</t>
+  </si>
+  <si>
+    <t>Galileo was an Italian astronomer who:</t>
+  </si>
+  <si>
+    <t> Developed the telescope</t>
+  </si>
+  <si>
+    <t>Discovered 4 satellites of Jupiter</t>
+  </si>
+  <si>
+    <t>Discovered that the movement of the pendulum produces a regular time measurement.</t>
+  </si>
+  <si>
+    <t>All are correct</t>
+  </si>
+  <si>
+    <t>Which country has always remained free from foreign rule?</t>
+  </si>
+  <si>
+    <t> Phillipines</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>What country's population had reached an estimated 60 million by the 1570s?</t>
   </si>
 </sst>
 </file>
@@ -404,27 +500,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="37.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.26953125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -450,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -462,10 +558,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -473,22 +569,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -496,22 +592,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -519,26 +615,163 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1947</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1951</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1956</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1971</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1970</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1966</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1984</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1977</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1">
-        <v>4</v>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Jnm8YDWSSFL5INu7WgSOuNLEkIYWrrOm9Hq+MP3MMuQUGVo09EXY/AsGwYq4/xAkMS1EerXoRX8mwFgmzrFAuA==" saltValue="WgYF5Vws4uPgbBnfHh0Vqw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>